<commit_message>
Made "U" a spare telemetry value.  Fixed unused motor count for "S" telemetry.
</commit_message>
<xml_diff>
--- a/serial_ICD.xlsx
+++ b/serial_ICD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>Commands</t>
   </si>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>U</t>
-  </si>
-  <si>
-    <t>read smoothed transmitter data</t>
   </si>
   <si>
     <t>V</t>
@@ -624,7 +621,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E15" sqref="E15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,14 +713,14 @@
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,7 +816,7 @@
         <v>55</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -863,11 +860,11 @@
         <v>25</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>61</v>
+      <c r="F15" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -880,10 +877,10 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,10 +893,10 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -908,10 +905,10 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -920,11 +917,11 @@
         <v>35</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>36</v>
@@ -943,7 +940,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -956,10 +953,10 @@
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,13 +964,13 @@
         <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -984,10 +981,10 @@
         <v>9</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1000,10 +997,10 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added battery monitor and altitude hold EEPROM variables. Restructured SerialComm.ino for more intuitive naming of commands/telemetry.  New names are recorded in SerialComm ICD.
</commit_message>
<xml_diff>
--- a/serial_ICD.xlsx
+++ b/serial_ICD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="-15" windowWidth="10725" windowHeight="9495"/>
+    <workbookView xWindow="10755" yWindow="-15" windowWidth="10800" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
   <si>
     <t>Commands</t>
   </si>
@@ -30,9 +30,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>roll/pitch gyro PID</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>Spare</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>serial transfer enable</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -123,18 +114,12 @@
     <t>calibrate magnetometer</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>read camera values</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>read roll/pitch gyro PID</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -144,12 +129,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>read roll/pitch auto level PID</t>
-  </si>
-  <si>
-    <t>roll/pitch auto level PID</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -204,9 +183,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>read raw transmitter data</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -240,15 +216,9 @@
     <t>read magnetometer cal values</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>vehicle attitude</t>
   </si>
   <si>
-    <t>accel calibration values</t>
-  </si>
-  <si>
     <t>read accel calibration values</t>
   </si>
   <si>
@@ -258,10 +228,94 @@
     <t>camera values</t>
   </si>
   <si>
-    <t>accel bias</t>
-  </si>
-  <si>
     <t>read raw magnetometer values</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>generate accel bias</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>custom debug messages</t>
+  </si>
+  <si>
+    <t>roll/pitch attitude mode PID</t>
+  </si>
+  <si>
+    <t>roll/pitch rate mode PID</t>
+  </si>
+  <si>
+    <t>calibrate accels</t>
+  </si>
+  <si>
+    <t>read roll/pitch rate mode PID</t>
+  </si>
+  <si>
+    <t>read roll/pitch attitude mode PID</t>
+  </si>
+  <si>
+    <t>battery monitor</t>
+  </si>
+  <si>
+    <t>read battery monitor settings</t>
   </si>
 </sst>
 </file>
@@ -277,18 +331,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -303,16 +351,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -618,401 +662,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
+      <c r="A1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="C14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5" t="s">
+      <c r="C16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5">
-        <v>3</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5">
-        <v>4</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5">
-        <v>5</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5">
-        <v>6</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>81</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>73</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>3</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="1">
+        <v>6</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <v>5</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="128" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
multiple bug fixes to serialComm for Configurator
</commit_message>
<xml_diff>
--- a/serial_ICD.xlsx
+++ b/serial_ICD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
   <si>
     <t>Commands</t>
   </si>
@@ -63,9 +63,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>transmitter calibration</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>read transmitter calibration</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -316,6 +310,24 @@
   </si>
   <si>
     <t>read battery monitor settings</t>
+  </si>
+  <si>
+    <t>waypoints</t>
+  </si>
+  <si>
+    <t>read waypoints</t>
+  </si>
+  <si>
+    <t>transmitter slope cal</t>
+  </si>
+  <si>
+    <t>transmitter offset cal</t>
+  </si>
+  <si>
+    <t>read transmitter slope values</t>
+  </si>
+  <si>
+    <t>read transmitter offset values</t>
   </si>
 </sst>
 </file>
@@ -665,7 +677,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,30 +716,30 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,26 +752,26 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -772,26 +784,26 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -800,30 +812,30 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -832,30 +844,30 @@
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,30 +876,30 @@
         <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,30 +908,30 @@
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,141 +939,149 @@
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="E25" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,13 +1089,13 @@
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1083,13 +1103,13 @@
         <v>2</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1097,13 +1117,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,13 +1131,13 @@
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E32" s="1">
         <v>6</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -1125,7 +1145,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many fix, unit test as INO, altitude hold with sonar, NOT YET WORKING
</commit_message>
<xml_diff>
--- a/serial_ICD.xlsx
+++ b/serial_ICD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="-15" windowWidth="10725" windowHeight="9495"/>
+    <workbookView xWindow="10755" yWindow="-15" windowWidth="10800" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
   <si>
     <t>Commands</t>
   </si>
@@ -30,9 +30,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>roll/pitch gyro PID</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>Spare</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>O</t>
   </si>
   <si>
-    <t>transmitter calibration</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -102,9 +93,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>serial transfer enable</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -123,18 +111,12 @@
     <t>calibrate magnetometer</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>read camera values</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>read roll/pitch gyro PID</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -144,12 +126,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>read roll/pitch auto level PID</t>
-  </si>
-  <si>
-    <t>roll/pitch auto level PID</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -174,9 +150,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>read transmitter calibration</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -201,15 +174,9 @@
     <t>U</t>
   </si>
   <si>
-    <t>read smoothed transmitter data</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
-    <t>read raw transmitter data</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -243,15 +210,9 @@
     <t>read magnetometer cal values</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>vehicle attitude</t>
   </si>
   <si>
-    <t>accel calibration values</t>
-  </si>
-  <si>
     <t>read accel calibration values</t>
   </si>
   <si>
@@ -261,10 +222,112 @@
     <t>camera values</t>
   </si>
   <si>
-    <t>accel bias</t>
-  </si>
-  <si>
     <t>read raw magnetometer values</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>generate accel bias</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>custom debug messages</t>
+  </si>
+  <si>
+    <t>roll/pitch attitude mode PID</t>
+  </si>
+  <si>
+    <t>roll/pitch rate mode PID</t>
+  </si>
+  <si>
+    <t>calibrate accels</t>
+  </si>
+  <si>
+    <t>read roll/pitch rate mode PID</t>
+  </si>
+  <si>
+    <t>read roll/pitch attitude mode PID</t>
+  </si>
+  <si>
+    <t>battery monitor</t>
+  </si>
+  <si>
+    <t>read battery monitor settings</t>
+  </si>
+  <si>
+    <t>waypoints</t>
+  </si>
+  <si>
+    <t>read waypoints</t>
+  </si>
+  <si>
+    <t>transmitter slope cal</t>
+  </si>
+  <si>
+    <t>transmitter offset cal</t>
+  </si>
+  <si>
+    <t>read transmitter slope values</t>
+  </si>
+  <si>
+    <t>read transmitter offset values</t>
   </si>
 </sst>
 </file>
@@ -280,18 +343,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -306,16 +363,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -621,401 +674,483 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
+      <c r="A1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="C14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5" t="s">
+      <c r="F18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5">
-        <v>3</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5">
-        <v>4</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5">
-        <v>5</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5">
-        <v>6</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>74</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>3</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="1">
+        <v>6</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <v>5</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="128" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>